<commit_message>
Fixed bug. P/L did not take into account fees.
</commit_message>
<xml_diff>
--- a/BackTesting Results/Statistics.xlsx
+++ b/BackTesting Results/Statistics.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\BackTesting Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB1D3A2-7406-4814-A10C-B6026C0DA74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Symbol</t>
   </si>
@@ -82,53 +76,23 @@
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>ETHUSD</t>
-  </si>
-  <si>
-    <t>DOTUSDT</t>
-  </si>
-  <si>
-    <t>BTCUSD</t>
-  </si>
-  <si>
-    <t>ADAUSDT</t>
-  </si>
-  <si>
     <t>2021-10-01</t>
   </si>
   <si>
-    <t>2021-07-01</t>
-  </si>
-  <si>
     <t>2021-11-30</t>
   </si>
   <si>
-    <t>2021-12-31</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
     <t>50.0%</t>
-  </si>
-  <si>
-    <t>57.6%</t>
-  </si>
-  <si>
-    <t>61.6%</t>
-  </si>
-  <si>
-    <t>52.9%</t>
-  </si>
-  <si>
-    <t>56.6%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,13 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -194,14 +155,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -248,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,27 +233,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,24 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,36 +442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -613,7 +508,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -621,13 +516,13 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
       </c>
       <c r="F2">
         <v>10000</v>
@@ -639,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="J2">
         <v>15</v>
@@ -650,8 +545,8 @@
       <c r="L2">
         <v>30</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>29</v>
+      <c r="M2" t="s">
+        <v>23</v>
       </c>
       <c r="N2">
         <v>-2</v>
@@ -666,246 +561,10 @@
         <v>-1500</v>
       </c>
       <c r="R2">
-        <v>451.08749999999998</v>
+        <v>451.0875</v>
       </c>
       <c r="S2">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3">
-        <v>10000</v>
-      </c>
-      <c r="G3">
-        <v>1.5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J3">
-        <v>49</v>
-      </c>
-      <c r="K3">
-        <v>36</v>
-      </c>
-      <c r="L3">
-        <v>85</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3">
-        <v>-1</v>
-      </c>
-      <c r="O3">
-        <v>14</v>
-      </c>
-      <c r="P3">
-        <v>7350</v>
-      </c>
-      <c r="Q3">
-        <v>-3600</v>
-      </c>
-      <c r="R3">
-        <v>1277.0625</v>
-      </c>
-      <c r="S3">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>10000</v>
-      </c>
-      <c r="G4">
-        <v>1.5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J4">
-        <v>69</v>
-      </c>
-      <c r="K4">
-        <v>43</v>
-      </c>
-      <c r="L4">
-        <v>112</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>26</v>
-      </c>
-      <c r="P4">
-        <v>10350</v>
-      </c>
-      <c r="Q4">
-        <v>-4300</v>
-      </c>
-      <c r="R4">
-        <v>1683.5625</v>
-      </c>
-      <c r="S4">
-        <v>6050</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5">
-        <v>10000</v>
-      </c>
-      <c r="G5">
-        <v>1.5</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J5">
-        <v>45</v>
-      </c>
-      <c r="K5">
-        <v>40</v>
-      </c>
-      <c r="L5">
-        <v>85</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5">
-        <v>-3</v>
-      </c>
-      <c r="O5">
-        <v>5</v>
-      </c>
-      <c r="P5">
-        <v>6750</v>
-      </c>
-      <c r="Q5">
-        <v>-4000</v>
-      </c>
-      <c r="R5">
-        <v>1277.2874999999999</v>
-      </c>
-      <c r="S5">
-        <v>2750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6">
-        <v>10000</v>
-      </c>
-      <c r="G6">
-        <v>1.5</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J6">
-        <v>60</v>
-      </c>
-      <c r="K6">
-        <v>46</v>
-      </c>
-      <c r="L6">
-        <v>106</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6">
-        <v>-6</v>
-      </c>
-      <c r="O6">
-        <v>14</v>
-      </c>
-      <c r="P6">
-        <v>9000</v>
-      </c>
-      <c r="Q6">
-        <v>-4600</v>
-      </c>
-      <c r="R6">
-        <v>1590.450000000001</v>
-      </c>
-      <c r="S6">
-        <v>4400</v>
+        <v>298.9125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>